<commit_message>
add reg/unreg batch file
</commit_message>
<xml_diff>
--- a/TestFirstRTD.xlsx
+++ b/TestFirstRTD.xlsx
@@ -86,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -107,32 +108,32 @@
   <volType type="realTimeData">
     <main first="kgi.tw.der.pricertdserver.2">
       <tp>
-        <v>8022.1888720707984</v>
+        <v>8132.3745035218917</v>
         <stp/>
         <stp>TSE00</stp>
         <tr r="A2" s="1"/>
         <tr r="C2" s="1"/>
       </tp>
       <tp>
-        <v>949.56809746206488</v>
+        <v>966.01417359622781</v>
         <stp/>
         <stp>TSE13</stp>
+        <tr r="C4" s="1"/>
         <tr r="A4" s="1"/>
-        <tr r="C4" s="1"/>
       </tp>
       <tp>
-        <v>293.3344546850887</v>
+        <v>295.67204537668647</v>
         <stp/>
         <stp>TSE26</stp>
+        <tr r="C5" s="1"/>
         <tr r="A5" s="1"/>
-        <tr r="C5" s="1"/>
       </tp>
       <tp>
-        <v>11095.625024755453</v>
+        <v>11318.035649166715</v>
         <stp/>
         <stp>TSE33</stp>
+        <tr r="C3" s="1"/>
         <tr r="A3" s="1"/>
-        <tr r="C3" s="1"/>
       </tp>
     </main>
   </volType>
@@ -429,14 +430,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.75" customWidth="1"/>
     <col min="2" max="2" width="11.125" customWidth="1"/>
-    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,55 +452,55 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,"TSE00")</f>
-        <v>8022.1888720707984</v>
+        <v>8132.3745035218917</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,B2)</f>
-        <v>8022.1888720707984</v>
+        <v>8132.3745035218917</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,"TSE33")</f>
-        <v>11095.625024755453</v>
+        <v>11318.035649166715</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,B3)</f>
-        <v>11095.625024755453</v>
+        <v>11318.035649166715</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,"TSE13")</f>
-        <v>949.56809746206488</v>
+        <v>966.01417359622781</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,B4)</f>
-        <v>949.56809746206488</v>
+        <v>966.01417359622781</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,"TSE26")</f>
-        <v>293.3344546850887</v>
+        <v>295.67204537668647</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>RTD("kgi.tw.der.pricertdserver.2",,B5)</f>
-        <v>293.3344546850887</v>
+        <v>295.67204537668647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>